<commit_message>
Adds resource correction flow
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gtp_100a.xlsx
+++ b/premise_gwp/data/lcia_gtp_100a.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>soil::unspecified</t>
+  </si>
+  <si>
+    <t>Carbon dioxide, non-fossil, resource correction</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C218"/>
+      <selection activeCell="V8" sqref="V8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -602,10 +605,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -616,7 +619,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -627,7 +630,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -638,7 +641,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -649,7 +652,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -657,10 +660,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -671,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -682,7 +685,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -693,7 +696,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -704,7 +707,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -712,10 +715,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -726,7 +729,7 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -737,7 +740,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -748,7 +751,7 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -759,7 +762,7 @@
         <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -770,7 +773,7 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -778,13 +781,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C19">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,7 +795,7 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -803,7 +806,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -814,7 +817,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -822,13 +825,13 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C23">
-        <v>1.9578</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -836,7 +839,7 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>1.9578</v>
@@ -847,7 +850,7 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25">
         <v>1.9578</v>
@@ -858,7 +861,7 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26">
         <v>1.9578</v>
@@ -869,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27">
         <v>1.9578</v>
@@ -877,10 +880,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C28">
         <v>1.9578</v>
@@ -891,7 +894,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29">
         <v>1.9578</v>
@@ -902,7 +905,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C30">
         <v>1.9578</v>
@@ -913,7 +916,7 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31">
         <v>1.9578</v>
@@ -924,7 +927,7 @@
         <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32">
         <v>1.9578</v>
@@ -935,7 +938,7 @@
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33">
         <v>1.9578</v>
@@ -943,13 +946,13 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34">
-        <v>0.38640000000000002</v>
+        <v>1.9578</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -957,7 +960,7 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>0.38640000000000002</v>
@@ -968,7 +971,7 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36">
         <v>0.38640000000000002</v>
@@ -979,7 +982,7 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37">
         <v>0.38640000000000002</v>
@@ -990,7 +993,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C38">
         <v>0.38640000000000002</v>
@@ -998,13 +1001,13 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39">
-        <v>2.26099103</v>
+        <v>0.38640000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C40">
         <v>2.26099103</v>
@@ -1023,7 +1026,7 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C41">
         <v>2.26099103</v>
@@ -1034,7 +1037,7 @@
         <v>11</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42">
         <v>2.26099103</v>
@@ -1045,7 +1048,7 @@
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43">
         <v>2.26099103</v>
@@ -1053,13 +1056,13 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44">
-        <v>234.2</v>
+        <v>2.26099103</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1067,7 +1070,7 @@
         <v>12</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C45">
         <v>234.2</v>
@@ -1078,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46">
         <v>234.2</v>
@@ -1089,7 +1092,7 @@
         <v>12</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47">
         <v>234.2</v>
@@ -1100,7 +1103,7 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48">
         <v>234.2</v>
@@ -1108,13 +1111,13 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49">
-        <v>200.74820020999999</v>
+        <v>234.2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1122,7 +1125,7 @@
         <v>13</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C50">
         <v>200.74820020999999</v>
@@ -1133,7 +1136,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51">
         <v>200.74820020999999</v>
@@ -1144,7 +1147,7 @@
         <v>13</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C52">
         <v>200.74820020999999</v>
@@ -1155,7 +1158,7 @@
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53">
         <v>200.74820020999999</v>
@@ -1163,13 +1166,13 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54">
-        <v>22.33931669</v>
+        <v>200.74820020999999</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,7 +1180,7 @@
         <v>14</v>
       </c>
       <c r="B55" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C55">
         <v>22.33931669</v>
@@ -1188,7 +1191,7 @@
         <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56">
         <v>22.33931669</v>
@@ -1199,7 +1202,7 @@
         <v>14</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C57">
         <v>22.33931669</v>
@@ -1210,7 +1213,7 @@
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C58">
         <v>22.33931669</v>
@@ -1218,13 +1221,13 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59">
-        <v>2504.5411716100002</v>
+        <v>22.33931669</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1232,7 +1235,7 @@
         <v>15</v>
       </c>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C60">
         <v>2504.5411716100002</v>
@@ -1243,7 +1246,7 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C61">
         <v>2504.5411716100002</v>
@@ -1254,7 +1257,7 @@
         <v>15</v>
       </c>
       <c r="B62" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C62">
         <v>2504.5411716100002</v>
@@ -1265,7 +1268,7 @@
         <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C63">
         <v>2504.5411716100002</v>
@@ -1273,13 +1276,13 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C64">
-        <v>4473.6284437100003</v>
+        <v>2504.5411716100002</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1287,7 +1290,7 @@
         <v>16</v>
       </c>
       <c r="B65" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C65">
         <v>4473.6284437100003</v>
@@ -1298,7 +1301,7 @@
         <v>16</v>
       </c>
       <c r="B66" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C66">
         <v>4473.6284437100003</v>
@@ -1309,7 +1312,7 @@
         <v>16</v>
       </c>
       <c r="B67" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67">
         <v>4473.6284437100003</v>
@@ -1320,7 +1323,7 @@
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C68">
         <v>4473.6284437100003</v>
@@ -1328,13 +1331,13 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C69">
-        <v>111.36886022</v>
+        <v>4473.6284437100003</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1342,7 +1345,7 @@
         <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C70">
         <v>111.36886022</v>
@@ -1353,7 +1356,7 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C71">
         <v>111.36886022</v>
@@ -1364,7 +1367,7 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C72">
         <v>111.36886022</v>
@@ -1375,7 +1378,7 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C73">
         <v>111.36886022</v>
@@ -1383,13 +1386,13 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C74">
-        <v>19.015345780000001</v>
+        <v>111.36886022</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -1397,7 +1400,7 @@
         <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C75">
         <v>19.015345780000001</v>
@@ -1408,7 +1411,7 @@
         <v>18</v>
       </c>
       <c r="B76" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C76">
         <v>19.015345780000001</v>
@@ -1419,7 +1422,7 @@
         <v>18</v>
       </c>
       <c r="B77" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C77">
         <v>19.015345780000001</v>
@@ -1430,7 +1433,7 @@
         <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C78">
         <v>19.015345780000001</v>
@@ -1438,13 +1441,13 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B79" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C79">
-        <v>0.12375371</v>
+        <v>19.015345780000001</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,7 +1455,7 @@
         <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C80">
         <v>0.12375371</v>
@@ -1463,7 +1466,7 @@
         <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C81">
         <v>0.12375371</v>
@@ -1474,7 +1477,7 @@
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C82">
         <v>0.12375371</v>
@@ -1485,7 +1488,7 @@
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C83">
         <v>0.12375371</v>
@@ -1493,13 +1496,13 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C84">
-        <v>8553.1856565500002</v>
+        <v>0.12375371</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,7 +1510,7 @@
         <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C85">
         <v>8553.1856565500002</v>
@@ -1518,7 +1521,7 @@
         <v>20</v>
       </c>
       <c r="B86" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C86">
         <v>8553.1856565500002</v>
@@ -1529,7 +1532,7 @@
         <v>20</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C87">
         <v>8553.1856565500002</v>
@@ -1540,7 +1543,7 @@
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C88">
         <v>8553.1856565500002</v>
@@ -1548,13 +1551,13 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B89" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C89">
-        <v>355.70904261999999</v>
+        <v>8553.1856565500002</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,7 +1565,7 @@
         <v>21</v>
       </c>
       <c r="B90" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C90">
         <v>355.70904261999999</v>
@@ -1573,7 +1576,7 @@
         <v>21</v>
       </c>
       <c r="B91" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C91">
         <v>355.70904261999999</v>
@@ -1584,7 +1587,7 @@
         <v>21</v>
       </c>
       <c r="B92" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C92">
         <v>355.70904261999999</v>
@@ -1595,7 +1598,7 @@
         <v>21</v>
       </c>
       <c r="B93" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C93">
         <v>355.70904261999999</v>
@@ -1603,13 +1606,13 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C94">
-        <v>10.96555186</v>
+        <v>355.70904261999999</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -1617,7 +1620,7 @@
         <v>22</v>
       </c>
       <c r="B95" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C95">
         <v>10.96555186</v>
@@ -1628,7 +1631,7 @@
         <v>22</v>
       </c>
       <c r="B96" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C96">
         <v>10.96555186</v>
@@ -1639,7 +1642,7 @@
         <v>22</v>
       </c>
       <c r="B97" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C97">
         <v>10.96555186</v>
@@ -1650,7 +1653,7 @@
         <v>22</v>
       </c>
       <c r="B98" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C98">
         <v>10.96555186</v>
@@ -1658,13 +1661,13 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C99">
-        <v>73.674216849999993</v>
+        <v>10.96555186</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -1672,7 +1675,7 @@
         <v>23</v>
       </c>
       <c r="B100" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C100">
         <v>73.674216849999993</v>
@@ -1683,7 +1686,7 @@
         <v>23</v>
       </c>
       <c r="B101" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C101">
         <v>73.674216849999993</v>
@@ -1694,7 +1697,7 @@
         <v>23</v>
       </c>
       <c r="B102" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C102">
         <v>73.674216849999993</v>
@@ -1705,7 +1708,7 @@
         <v>23</v>
       </c>
       <c r="B103" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C103">
         <v>73.674216849999993</v>
@@ -1713,13 +1716,13 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B104" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C104">
-        <v>8977.0146687300003</v>
+        <v>73.674216849999993</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -1727,7 +1730,7 @@
         <v>24</v>
       </c>
       <c r="B105" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C105">
         <v>8977.0146687300003</v>
@@ -1738,7 +1741,7 @@
         <v>24</v>
       </c>
       <c r="B106" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C106">
         <v>8977.0146687300003</v>
@@ -1749,7 +1752,7 @@
         <v>24</v>
       </c>
       <c r="B107" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C107">
         <v>8977.0146687300003</v>
@@ -1760,7 +1763,7 @@
         <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C108">
         <v>8977.0146687300003</v>
@@ -1768,13 +1771,13 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C109">
-        <v>13455.63285373</v>
+        <v>8977.0146687300003</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -1782,7 +1785,7 @@
         <v>25</v>
       </c>
       <c r="B110" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C110">
         <v>13455.63285373</v>
@@ -1793,7 +1796,7 @@
         <v>25</v>
       </c>
       <c r="B111" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C111">
         <v>13455.63285373</v>
@@ -1804,7 +1807,7 @@
         <v>25</v>
       </c>
       <c r="B112" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C112">
         <v>13455.63285373</v>
@@ -1815,7 +1818,7 @@
         <v>25</v>
       </c>
       <c r="B113" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C113">
         <v>13455.63285373</v>
@@ -1823,13 +1826,13 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B114" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C114">
-        <v>967.40161765000005</v>
+        <v>13455.63285373</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -1837,7 +1840,7 @@
         <v>26</v>
       </c>
       <c r="B115" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C115">
         <v>967.40161765000005</v>
@@ -1848,7 +1851,7 @@
         <v>26</v>
       </c>
       <c r="B116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C116">
         <v>967.40161765000005</v>
@@ -1859,7 +1862,7 @@
         <v>26</v>
       </c>
       <c r="B117" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C117">
         <v>967.40161765000005</v>
@@ -1870,7 +1873,7 @@
         <v>26</v>
       </c>
       <c r="B118" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C118">
         <v>967.40161765000005</v>
@@ -1878,24 +1881,24 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B119" t="s">
         <v>54</v>
       </c>
       <c r="C119">
-        <v>5.6999999999999993</v>
+        <v>967.40161765000005</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B120" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C120">
-        <v>0.32489626999999999</v>
+        <v>5.6999999999999993</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -1903,7 +1906,7 @@
         <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C121">
         <v>0.32489626999999999</v>
@@ -1914,7 +1917,7 @@
         <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C122">
         <v>0.32489626999999999</v>
@@ -1925,7 +1928,7 @@
         <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C123">
         <v>0.32489626999999999</v>
@@ -1936,7 +1939,7 @@
         <v>28</v>
       </c>
       <c r="B124" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C124">
         <v>0.32489626999999999</v>
@@ -1944,13 +1947,13 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B125" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C125">
-        <v>296.86626878999999</v>
+        <v>0.32489626999999999</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -1958,7 +1961,7 @@
         <v>29</v>
       </c>
       <c r="B126" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C126">
         <v>296.86626878999999</v>
@@ -1969,7 +1972,7 @@
         <v>29</v>
       </c>
       <c r="B127" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C127">
         <v>296.86626878999999</v>
@@ -1980,7 +1983,7 @@
         <v>29</v>
       </c>
       <c r="B128" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C128">
         <v>296.86626878999999</v>
@@ -1991,7 +1994,7 @@
         <v>29</v>
       </c>
       <c r="B129" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C129">
         <v>296.86626878999999</v>
@@ -1999,13 +2002,13 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B130" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C130">
-        <v>4167.5190047699998</v>
+        <v>296.86626878999999</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -2013,7 +2016,7 @@
         <v>30</v>
       </c>
       <c r="B131" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C131">
         <v>4167.5190047699998</v>
@@ -2024,7 +2027,7 @@
         <v>30</v>
       </c>
       <c r="B132" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C132">
         <v>4167.5190047699998</v>
@@ -2035,7 +2038,7 @@
         <v>30</v>
       </c>
       <c r="B133" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C133">
         <v>4167.5190047699998</v>
@@ -2046,7 +2049,7 @@
         <v>30</v>
       </c>
       <c r="B134" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C134">
         <v>4167.5190047699998</v>
@@ -2054,13 +2057,13 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B135" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C135">
-        <v>261.70622477000001</v>
+        <v>4167.5190047699998</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -2068,7 +2071,7 @@
         <v>31</v>
       </c>
       <c r="B136" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C136">
         <v>261.70622477000001</v>
@@ -2079,7 +2082,7 @@
         <v>31</v>
       </c>
       <c r="B137" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C137">
         <v>261.70622477000001</v>
@@ -2090,7 +2093,7 @@
         <v>31</v>
       </c>
       <c r="B138" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C138">
         <v>261.70622477000001</v>
@@ -2101,7 +2104,7 @@
         <v>31</v>
       </c>
       <c r="B139" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C139">
         <v>261.70622477000001</v>
@@ -2109,13 +2112,13 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B140" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C140">
-        <v>15922.81568973</v>
+        <v>261.70622477000001</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
@@ -2123,7 +2126,7 @@
         <v>32</v>
       </c>
       <c r="B141" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C141">
         <v>15922.81568973</v>
@@ -2134,7 +2137,7 @@
         <v>32</v>
       </c>
       <c r="B142" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C142">
         <v>15922.81568973</v>
@@ -2145,7 +2148,7 @@
         <v>32</v>
       </c>
       <c r="B143" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C143">
         <v>15922.81568973</v>
@@ -2156,7 +2159,7 @@
         <v>32</v>
       </c>
       <c r="B144" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C144">
         <v>15922.81568973</v>
@@ -2164,13 +2167,13 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C145">
-        <v>1.22891799</v>
+        <v>15922.81568973</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -2178,7 +2181,7 @@
         <v>33</v>
       </c>
       <c r="B146" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C146">
         <v>1.22891799</v>
@@ -2189,7 +2192,7 @@
         <v>33</v>
       </c>
       <c r="B147" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C147">
         <v>1.22891799</v>
@@ -2200,7 +2203,7 @@
         <v>33</v>
       </c>
       <c r="B148" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C148">
         <v>1.22891799</v>
@@ -2211,7 +2214,7 @@
         <v>33</v>
       </c>
       <c r="B149" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C149">
         <v>1.22891799</v>
@@ -2219,13 +2222,13 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B150" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C150">
-        <v>8448.3513268099996</v>
+        <v>1.22891799</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -2233,7 +2236,7 @@
         <v>34</v>
       </c>
       <c r="B151" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C151">
         <v>8448.3513268099996</v>
@@ -2244,7 +2247,7 @@
         <v>34</v>
       </c>
       <c r="B152" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C152">
         <v>8448.3513268099996</v>
@@ -2255,7 +2258,7 @@
         <v>34</v>
       </c>
       <c r="B153" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C153">
         <v>8448.3513268099996</v>
@@ -2266,7 +2269,7 @@
         <v>34</v>
       </c>
       <c r="B154" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C154">
         <v>8448.3513268099996</v>
@@ -2274,13 +2277,13 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B155" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C155">
-        <v>20.422240250000002</v>
+        <v>8448.3513268099996</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -2288,7 +2291,7 @@
         <v>35</v>
       </c>
       <c r="B156" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C156">
         <v>20.422240250000002</v>
@@ -2299,7 +2302,7 @@
         <v>35</v>
       </c>
       <c r="B157" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C157">
         <v>20.422240250000002</v>
@@ -2310,7 +2313,7 @@
         <v>35</v>
       </c>
       <c r="B158" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C158">
         <v>20.422240250000002</v>
@@ -2321,7 +2324,7 @@
         <v>35</v>
       </c>
       <c r="B159" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C159">
         <v>20.422240250000002</v>
@@ -2329,13 +2332,13 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B160" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C160">
-        <v>94.493668409999998</v>
+        <v>20.422240250000002</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -2343,7 +2346,7 @@
         <v>36</v>
       </c>
       <c r="B161" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C161">
         <v>94.493668409999998</v>
@@ -2354,7 +2357,7 @@
         <v>36</v>
       </c>
       <c r="B162" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C162">
         <v>94.493668409999998</v>
@@ -2365,7 +2368,7 @@
         <v>36</v>
       </c>
       <c r="B163" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C163">
         <v>94.493668409999998</v>
@@ -2376,7 +2379,7 @@
         <v>36</v>
       </c>
       <c r="B164" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C164">
         <v>94.493668409999998</v>
@@ -2384,13 +2387,13 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B165" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C165">
-        <v>5.6999999999999993</v>
+        <v>94.493668409999998</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -2398,7 +2401,7 @@
         <v>37</v>
       </c>
       <c r="B166" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C166">
         <v>5.6999999999999993</v>
@@ -2409,7 +2412,7 @@
         <v>37</v>
       </c>
       <c r="B167" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C167">
         <v>5.6999999999999993</v>
@@ -2420,7 +2423,7 @@
         <v>37</v>
       </c>
       <c r="B168" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C168">
         <v>5.6999999999999993</v>
@@ -2431,7 +2434,7 @@
         <v>37</v>
       </c>
       <c r="B169" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C169">
         <v>5.6999999999999993</v>
@@ -2439,10 +2442,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B170" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C170">
         <v>5.6999999999999993</v>
@@ -2453,7 +2456,7 @@
         <v>38</v>
       </c>
       <c r="B171" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C171">
         <v>5.6999999999999993</v>
@@ -2464,7 +2467,7 @@
         <v>38</v>
       </c>
       <c r="B172" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C172">
         <v>5.6999999999999993</v>
@@ -2475,7 +2478,7 @@
         <v>38</v>
       </c>
       <c r="B173" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C173">
         <v>5.6999999999999993</v>
@@ -2486,7 +2489,7 @@
         <v>38</v>
       </c>
       <c r="B174" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C174">
         <v>5.6999999999999993</v>
@@ -2497,7 +2500,7 @@
         <v>38</v>
       </c>
       <c r="B175" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C175">
         <v>5.6999999999999993</v>
@@ -2505,13 +2508,13 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B176" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C176">
-        <v>1.6819777499999999</v>
+        <v>5.6999999999999993</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -2519,7 +2522,7 @@
         <v>39</v>
       </c>
       <c r="B177" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C177">
         <v>1.6819777499999999</v>
@@ -2530,7 +2533,7 @@
         <v>39</v>
       </c>
       <c r="B178" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C178">
         <v>1.6819777499999999</v>
@@ -2541,7 +2544,7 @@
         <v>39</v>
       </c>
       <c r="B179" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C179">
         <v>1.6819777499999999</v>
@@ -2552,7 +2555,7 @@
         <v>39</v>
       </c>
       <c r="B180" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C180">
         <v>1.6819777499999999</v>
@@ -2560,13 +2563,13 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B181" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C181">
-        <v>4.3</v>
+        <v>1.6819777499999999</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -2574,7 +2577,7 @@
         <v>40</v>
       </c>
       <c r="B182" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C182">
         <v>4.3</v>
@@ -2585,7 +2588,7 @@
         <v>40</v>
       </c>
       <c r="B183" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C183">
         <v>4.3</v>
@@ -2596,7 +2599,7 @@
         <v>40</v>
       </c>
       <c r="B184" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C184">
         <v>4.3</v>
@@ -2607,7 +2610,7 @@
         <v>40</v>
       </c>
       <c r="B185" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C185">
         <v>4.3</v>
@@ -2615,13 +2618,13 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B186" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C186">
-        <v>479.24856327999998</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
@@ -2629,7 +2632,7 @@
         <v>41</v>
       </c>
       <c r="B187" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C187">
         <v>479.24856327999998</v>
@@ -2640,7 +2643,7 @@
         <v>41</v>
       </c>
       <c r="B188" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C188">
         <v>479.24856327999998</v>
@@ -2651,7 +2654,7 @@
         <v>41</v>
       </c>
       <c r="B189" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C189">
         <v>479.24856327999998</v>
@@ -2662,7 +2665,7 @@
         <v>41</v>
       </c>
       <c r="B190" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C190">
         <v>479.24856327999998</v>
@@ -2670,13 +2673,13 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B191" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C191">
-        <v>8038.4037214299997</v>
+        <v>479.24856327999998</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
@@ -2684,7 +2687,7 @@
         <v>42</v>
       </c>
       <c r="B192" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C192">
         <v>8038.4037214299997</v>
@@ -2695,7 +2698,7 @@
         <v>42</v>
       </c>
       <c r="B193" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C193">
         <v>8038.4037214299997</v>
@@ -2706,7 +2709,7 @@
         <v>42</v>
       </c>
       <c r="B194" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C194">
         <v>8038.4037214299997</v>
@@ -2717,7 +2720,7 @@
         <v>42</v>
       </c>
       <c r="B195" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C195">
         <v>8038.4037214299997</v>
@@ -2725,13 +2728,13 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B196" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C196">
-        <v>2335.1918620900001</v>
+        <v>8038.4037214299997</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -2739,7 +2742,7 @@
         <v>43</v>
       </c>
       <c r="B197" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C197">
         <v>2335.1918620900001</v>
@@ -2750,7 +2753,7 @@
         <v>43</v>
       </c>
       <c r="B198" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C198">
         <v>2335.1918620900001</v>
@@ -2761,7 +2764,7 @@
         <v>43</v>
       </c>
       <c r="B199" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C199">
         <v>2335.1918620900001</v>
@@ -2772,7 +2775,7 @@
         <v>43</v>
       </c>
       <c r="B200" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C200">
         <v>2335.1918620900001</v>
@@ -2780,13 +2783,13 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B201" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C201">
-        <v>12708.85603515</v>
+        <v>2335.1918620900001</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -2794,7 +2797,7 @@
         <v>44</v>
       </c>
       <c r="B202" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C202">
         <v>12708.85603515</v>
@@ -2805,7 +2808,7 @@
         <v>44</v>
       </c>
       <c r="B203" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C203">
         <v>12708.85603515</v>
@@ -2816,7 +2819,7 @@
         <v>44</v>
       </c>
       <c r="B204" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C204">
         <v>12708.85603515</v>
@@ -2827,7 +2830,7 @@
         <v>44</v>
       </c>
       <c r="B205" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C205">
         <v>12708.85603515</v>
@@ -2835,24 +2838,24 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B206" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C206">
-        <v>-2.8</v>
+        <v>12708.85603515</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B207" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C207">
-        <v>18118.785399789998</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -2860,7 +2863,7 @@
         <v>46</v>
       </c>
       <c r="B208" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C208">
         <v>18118.785399789998</v>
@@ -2871,7 +2874,7 @@
         <v>46</v>
       </c>
       <c r="B209" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C209">
         <v>18118.785399789998</v>
@@ -2882,7 +2885,7 @@
         <v>46</v>
       </c>
       <c r="B210" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C210">
         <v>18118.785399789998</v>
@@ -2893,7 +2896,7 @@
         <v>46</v>
       </c>
       <c r="B211" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C211">
         <v>18118.785399789998</v>
@@ -2901,24 +2904,24 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B212" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C212">
-        <v>10284.281800029999</v>
+        <v>18118.785399789998</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B213" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C213">
-        <v>28214.809302739999</v>
+        <v>10284.281800029999</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -2926,7 +2929,7 @@
         <v>48</v>
       </c>
       <c r="B214" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C214">
         <v>28214.809302739999</v>
@@ -2937,7 +2940,7 @@
         <v>48</v>
       </c>
       <c r="B215" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C215">
         <v>28214.809302739999</v>
@@ -2948,7 +2951,7 @@
         <v>48</v>
       </c>
       <c r="B216" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C216">
         <v>28214.809302739999</v>
@@ -2959,7 +2962,7 @@
         <v>48</v>
       </c>
       <c r="B217" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C217">
         <v>28214.809302739999</v>
@@ -2967,12 +2970,23 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
+        <v>48</v>
+      </c>
+      <c r="B218" t="s">
+        <v>54</v>
+      </c>
+      <c r="C218">
+        <v>28214.809302739999</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
         <v>49</v>
       </c>
-      <c r="B218" t="s">
-        <v>53</v>
-      </c>
-      <c r="C218">
+      <c r="B219" t="s">
+        <v>53</v>
+      </c>
+      <c r="C219">
         <v>0.66</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix CF for "carbon dioxide, resource correction"
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gtp_100a.xlsx
+++ b/premise_gwp/data/lcia_gtp_100a.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateCount="5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -573,7 +573,7 @@
   <dimension ref="A1:C219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -611,7 +611,7 @@
         <v>50</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>